<commit_message>
Fixed lecture figure paths so things are not overwritten.
</commit_message>
<xml_diff>
--- a/figure-creation/snow.xlsx
+++ b/figure-creation/snow.xlsx
@@ -471,7 +471,7 @@
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="1.5" style="4" customWidth="1"/>
     <col min="5" max="5" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -525,7 +525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:16" s="4" customFormat="1"/>
+    <row r="5" spans="2:16" s="4" customFormat="1" ht="7" customHeight="1"/>
     <row r="6" spans="2:16">
       <c r="B6" s="1">
         <v>1893</v>

</xml_diff>